<commit_message>
ETP input maps update
ETP as input maps is now available. Data source GLEAM v4.1 (2024).
</commit_message>
<xml_diff>
--- a/Generical_Input_Files/LULC_parameters.xlsx
+++ b/Generical_Input_Files/LULC_parameters.xlsx
@@ -1,40 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d29a325a694f12f3/Documentos/GitHub/HydroPol2D/Input_Data_Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\WadiLab_General\Study_cases\Marcus\South_America\Modelo_Amazonia_3k\HydroPol2D_Model\Input_Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_FD6EE03DC7E48B0ACDA3D68F4ACC87777E01122E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7EF7B8-E5E6-4342-A82E-81B144155992}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231AD906-EAAF-4F48-A46C-7DF995AE3A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LULC_parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={00BD003A-00BB-4411-85C4-000C005F00A2}</author>
-    <author>tc={00180020-0025-4331-A3CF-0082005700E1}</author>
-    <author>tc={00FC00E4-00ED-4C33-84A8-00A900FA0029}</author>
-    <author>tc={00E50033-0002-4046-AAC3-00DC00000067}</author>
-    <author>tc={00C0003D-002A-4900-A5C3-00B900B300AC}</author>
-    <author>tc={00700038-007E-4AD7-A700-00A4007400AE}</author>
-    <author>tc={004A00DA-00EB-47A7-A607-004200340047}</author>
-    <author>tc={009800E2-00B2-412F-9515-00FE00FC00F3}</author>
-    <author>tc={001A008F-00E9-4B94-A5A1-008700670056}</author>
-    <author>tc={00810027-00F9-4FDC-9CD3-0050002300B4}</author>
+    <author>tc={00F300C9-00DA-4FC0-A2C3-004D008100E6}</author>
+    <author>tc={00760080-0027-49A3-B215-006100CE0086}</author>
+    <author>tc={00EE00C1-00FD-45FF-8C41-009D00AF0085}</author>
+    <author>tc={00FC00D6-0018-4216-8F03-0043008E00EC}</author>
+    <author>tc={00E5007F-00B8-43FC-AA83-00C7001A0056}</author>
+    <author>tc={0014006D-0023-431A-A3C6-004F00C60070}</author>
+    <author>tc={009500C5-0020-40AE-A739-003900480080}</author>
+    <author>tc={009A00A3-007E-4049-AB2C-0095001B00DB}</author>
+    <author>tc={00FA0094-008B-4050-A250-00A600FD006D}</author>
+    <author>tc={00AD001B-009D-427C-BE3F-006600710035}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00BD003A-00BB-4411-85C4-000C005F00A2}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00F300C9-00DA-4FC0-A2C3-004D008100E6}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -43,7 +57,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00180020-0025-4331-A3CF-0082005700E1}">
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00760080-0027-49A3-B215-006100CE0086}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +66,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{00FC00E4-00ED-4C33-84A8-00A900FA0029}">
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{00EE00C1-00FD-45FF-8C41-009D00AF0085}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,7 +75,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{00E50033-0002-4046-AAC3-00DC00000067}">
+    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{00FC00D6-0018-4216-8F03-0043008E00EC}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +84,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{00C0003D-002A-4900-A5C3-00B900B300AC}">
+    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{00E5007F-00B8-43FC-AA83-00C7001A0056}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -79,7 +93,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{00700038-007E-4AD7-A700-00A4007400AE}">
+    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{0014006D-0023-431A-A3C6-004F00C60070}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +103,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="G2" authorId="6" shapeId="0" xr:uid="{004A00DA-00EB-47A7-A607-004200340047}">
+    <comment ref="G2" authorId="6" shapeId="0" xr:uid="{009500C5-0020-40AE-A739-003900480080}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -99,7 +113,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="H2" authorId="7" shapeId="0" xr:uid="{009800E2-00B2-412F-9515-00FE00FC00F3}">
+    <comment ref="H2" authorId="7" shapeId="0" xr:uid="{009A00A3-007E-4049-AB2C-0095001B00DB}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +122,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="I2" authorId="8" shapeId="0" xr:uid="{001A008F-00E9-4B94-A5A1-008700670056}">
+    <comment ref="I2" authorId="8" shapeId="0" xr:uid="{00FA0094-008B-4050-A250-00A600FD006D}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -117,7 +131,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="J2" authorId="9" shapeId="0" xr:uid="{00810027-00F9-4FDC-9CD3-0050002300B4}">
+    <comment ref="J2" authorId="9" shapeId="0" xr:uid="{00AD001B-009D-427C-BE3F-006600710035}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -131,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t xml:space="preserve">HydroPol2D - LULC Parameters </t>
   </si>
@@ -260,6 +274,12 @@
   </si>
   <si>
     <t>Snow and Ice</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>two waves</t>
   </si>
 </sst>
 </file>
@@ -301,7 +321,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +338,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -393,6 +419,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,7 +448,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Marcus" id="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" userId="" providerId=""/>
+  <person displayName="Marcus" id="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" userId="" providerId=""/>
 </personList>
 </file>
 
@@ -632,45 +662,45 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00BD003A-00BB-4411-85C4-000C005F00A2}">
+  <threadedComment ref="A2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00F300C9-00DA-4FC0-A2C3-004D008100E6}">
     <text xml:space="preserve">Enter the name of each land use in your LULC .TIF map.
 </text>
   </threadedComment>
-  <threadedComment ref="B2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00180020-0025-4331-A3CF-0082005700E1}">
+  <threadedComment ref="B2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00760080-0027-49A3-B215-006100CE0086}">
     <text xml:space="preserve">LULC index. Please enter positive integers. 0 is included and is typically assumed as water. 
 </text>
   </threadedComment>
-  <threadedComment ref="C2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00FC00E4-00ED-4C33-84A8-00A900FA0029}">
+  <threadedComment ref="C2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00EE00C1-00FD-45FF-8C41-009D00AF0085}">
     <text xml:space="preserve">Manning's roughness coefficient
 </text>
   </threadedComment>
-  <threadedComment ref="D2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00E50033-0002-4046-AAC3-00DC00000067}">
+  <threadedComment ref="D2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00FC00D6-0018-4216-8F03-0043008E00EC}">
     <text xml:space="preserve">Initial abstraction due to interception by plants or small reservoirs for each LULC
 </text>
   </threadedComment>
-  <threadedComment ref="E2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00C0003D-002A-4900-A5C3-00B900B300AC}">
+  <threadedComment ref="E2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00E5007F-00B8-43FC-AA83-00C7001A0056}">
     <text xml:space="preserve">In case you don't enter an input map for depths (i.e., warm-up depths), this is the initial water depth for each LULC
 </text>
   </threadedComment>
-  <threadedComment ref="F2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00700038-007E-4AD7-A700-00A4007400AE}">
+  <threadedComment ref="F2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{0014006D-0023-431A-A3C6-004F00C60070}">
     <text xml:space="preserve">C1 Build-up parameter, such that:
 B = C1*exp(-ADD*C2)
 </text>
   </threadedComment>
-  <threadedComment ref="G2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{004A00DA-00EB-47A7-A607-004200340047}">
+  <threadedComment ref="G2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{009500C5-0020-40AE-A739-003900480080}">
     <text xml:space="preserve">C2 Build-up exponent, such that:
 B = C1*exp(-ADD*C2)
 </text>
   </threadedComment>
-  <threadedComment ref="H2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{009800E2-00B2-412F-9515-00FE00FC00F3}">
+  <threadedComment ref="H2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{009A00A3-007E-4049-AB2C-0095001B00DB}">
     <text xml:space="preserve">C3 Wash-off parameter that can be used in the rating curve or in the traditional wash-off equation. To choose which wash-off function is used, you need to change the flag_wq_model in the general data
 </text>
   </threadedComment>
-  <threadedComment ref="I2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{001A008F-00E9-4B94-A5A1-008700670056}">
+  <threadedComment ref="I2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00FA0094-008B-4050-A250-00A600FD006D}">
     <text xml:space="preserve">C4 Wash-off parameter that can be used in the rating curve or in the traditional wash-off equation. To choose which wash-off function is used, you need to change the flag_wq_model in the general data
 </text>
   </threadedComment>
-  <threadedComment ref="J2" personId="{78C3D9D8-17E0-2F08-0C6A-210D1578C46A}" id="{00810027-00F9-4FDC-9CD3-0050002300B4}">
+  <threadedComment ref="J2" personId="{C3FC4D26-FB65-BDCA-044F-CEEBA72BA3DA}" id="{00AD001B-009D-427C-BE3F-006600710035}">
     <text xml:space="preserve">This is mandatory. The index associated with impervious areas are used in the model and infiltration is neglected for this LULC.
 </text>
   </threadedComment>
@@ -683,7 +713,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,19 +733,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -758,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>2.53E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D3" s="5">
         <v>0</v>
@@ -791,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>3.5000000000000003E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
@@ -822,7 +852,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5">
-        <v>3.2000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D5" s="5">
         <v>0</v>
@@ -853,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>3.2300000000000002E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="D6" s="5">
         <v>0</v>
@@ -884,7 +914,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="5">
-        <v>3.1600000000000003E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -915,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="5">
-        <v>3.32E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D8" s="5">
         <v>0</v>
@@ -946,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="5">
-        <v>2.98E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
@@ -977,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="5">
-        <v>2.0899999999999998E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="D10" s="5">
         <v>0</v>
@@ -1546,4 +1576,184 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="10">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E9" si="0">D2*2</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D9" s="10">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>